<commit_message>
updated components, added filtering and delete button
</commit_message>
<xml_diff>
--- a/T2 - Tabla puntuación.xlsx
+++ b/T2 - Tabla puntuación.xlsx
@@ -10,7 +10,6 @@
     <sheet name="PUNTUACIÓN" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>APLICACIÓN</t>
   </si>
@@ -127,13 +126,16 @@
   </si>
   <si>
     <t>MAQUETACIÓN RESPONSIVE GRID</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +184,13 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -356,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -438,6 +447,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -776,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D9:E12"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -790,7 +802,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:8" ht="15" thickBot="1"/>
-    <row r="2" spans="3:8" ht="14.45">
+    <row r="2" spans="3:8">
       <c r="C2" s="14" t="s">
         <v>19</v>
       </c>
@@ -800,7 +812,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" spans="3:8" ht="14.45">
+    <row r="3" spans="3:8">
       <c r="C3" s="17" t="s">
         <v>20</v>
       </c>
@@ -810,7 +822,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="3:8" ht="14.45">
+    <row r="4" spans="3:8">
       <c r="C4" s="17" t="s">
         <v>21</v>
       </c>
@@ -830,7 +842,7 @@
       <c r="G5" s="21"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" spans="3:8" ht="14.45">
+    <row r="6" spans="3:8">
       <c r="C6" s="23"/>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
@@ -864,56 +876,64 @@
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="25"/>
+      <c r="D9" s="25" t="s">
+        <v>32</v>
+      </c>
       <c r="E9" s="26"/>
       <c r="F9" s="3">
         <v>0.5</v>
       </c>
       <c r="G9" s="13">
         <f>COUNTIF(D9:E9,"=X")*0.5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" ht="14.45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8">
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="25" t="s">
+        <v>32</v>
+      </c>
       <c r="E10" s="26"/>
       <c r="F10" s="3">
         <v>0.5</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" ref="G10:G12" si="0">COUNTIF(D10:E10,"=X")*0.5</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="3:8">
       <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="25" t="s">
+        <v>32</v>
+      </c>
       <c r="E11" s="26"/>
       <c r="F11" s="3">
         <v>0.5</v>
       </c>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" ht="14.45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8">
       <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="25"/>
+      <c r="D12" s="25" t="s">
+        <v>32</v>
+      </c>
       <c r="E12" s="26"/>
       <c r="F12" s="3">
         <v>0.5</v>
       </c>
       <c r="G12" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="3:8">
@@ -927,10 +947,10 @@
       </c>
       <c r="G13" s="12">
         <f>MIN(2,SUM(G9:G12))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" ht="27.6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="25.5">
       <c r="C14" s="1"/>
       <c r="D14" s="10" t="s">
         <v>16</v>
@@ -973,46 +993,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="14.45">
+    <row r="17" spans="3:7">
       <c r="C17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="D17" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="F17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" ht="14.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
       <c r="C18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="F18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G18" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" ht="14.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
       <c r="C19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="F19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G19" s="13">
         <f>COUNTIF(D19:E19,"=X")*0.75</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="20" spans="3:7">
@@ -1026,10 +1058,10 @@
       </c>
       <c r="G20" s="12">
         <f>MIN(6,SUM(G15:G19))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" ht="27.6">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="25.5">
       <c r="C21" s="1"/>
       <c r="D21" s="10" t="s">
         <v>16</v>
@@ -1044,7 +1076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="3:7" ht="14.45">
+    <row r="22" spans="3:7">
       <c r="C22" s="7" t="s">
         <v>10</v>
       </c>
@@ -1058,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:7" ht="14.45">
+    <row r="23" spans="3:7">
       <c r="C23" s="7" t="s">
         <v>12</v>
       </c>
@@ -1072,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:7" ht="14.45">
+    <row r="24" spans="3:7">
       <c r="C24" s="7" t="s">
         <v>14</v>
       </c>
@@ -1086,21 +1118,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:7" ht="14.45">
+    <row r="25" spans="3:7">
       <c r="C25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="F25" s="3">
         <v>0.5</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:7" ht="14.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7">
       <c r="C26" s="7" t="s">
         <v>11</v>
       </c>
@@ -1118,17 +1154,19 @@
       <c r="C27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="30"/>
+      <c r="D27" s="30" t="s">
+        <v>32</v>
+      </c>
       <c r="E27" s="30"/>
       <c r="F27" s="3">
         <v>0.5</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:7" ht="14.45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7">
       <c r="C28" s="7" t="s">
         <v>13</v>
       </c>
@@ -1153,7 +1191,7 @@
       </c>
       <c r="G29" s="12">
         <f>MIN(2,SUM(G23:G28))</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="30" spans="3:7">
@@ -1165,7 +1203,7 @@
       <c r="F30" s="29"/>
       <c r="G30" s="8">
         <f>MIN(10,SUM(G29,G20,G13))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
subiendo cambios a front y backend para funcionamiento del front
</commit_message>
<xml_diff>
--- a/T2 - Tabla puntuación.xlsx
+++ b/T2 - Tabla puntuación.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="PUNTUACIÓN" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PUNTUACIÓN!$A$1:$H$31</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>APLICACIÓN</t>
   </si>
@@ -129,13 +132,16 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +425,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -447,9 +456,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -788,21 +794,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="3.5" customWidth="1"/>
     <col min="3" max="3" width="31.375" customWidth="1"/>
     <col min="4" max="4" width="12.125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="8" max="8" width="4.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" ht="15" thickBot="1"/>
-    <row r="2" spans="3:8">
+    <row r="1" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C2" s="14" t="s">
         <v>19</v>
       </c>
@@ -812,7 +819,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" spans="3:8">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C3" s="17" t="s">
         <v>20</v>
       </c>
@@ -822,7 +829,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="3:8">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C4" s="17" t="s">
         <v>21</v>
       </c>
@@ -832,7 +839,7 @@
       <c r="G4" s="18"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" spans="3:8" ht="15" thickBot="1">
+    <row r="5" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="19" t="s">
         <v>24</v>
       </c>
@@ -842,7 +849,7 @@
       <c r="G5" s="21"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" spans="3:8">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C6" s="23"/>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
@@ -850,21 +857,21 @@
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" spans="3:8" ht="15">
-      <c r="C7" s="31" t="s">
+    <row r="7" spans="3:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="C7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-    </row>
-    <row r="8" spans="3:8">
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="8" t="s">
         <v>4</v>
       </c>
@@ -872,14 +879,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="3:8">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="26"/>
+      <c r="D9" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="27"/>
       <c r="F9" s="3">
         <v>0.5</v>
       </c>
@@ -888,14 +895,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="3:8">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="26"/>
+      <c r="D10" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="27"/>
       <c r="F10" s="3">
         <v>0.5</v>
       </c>
@@ -904,14 +911,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="3:8">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="26"/>
+      <c r="D11" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="27"/>
       <c r="F11" s="3">
         <v>0.5</v>
       </c>
@@ -920,14 +927,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="3:8">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="26"/>
+      <c r="D12" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="27"/>
       <c r="F12" s="3">
         <v>0.5</v>
       </c>
@@ -936,7 +943,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="3:8">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C13" s="22" t="s">
         <v>27</v>
       </c>
@@ -950,7 +957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="3:8" ht="25.5">
+    <row r="14" spans="3:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
       <c r="D14" s="10" t="s">
         <v>16</v>
@@ -965,39 +972,47 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="3:8">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="F15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G15" s="13">
         <f>COUNTIF(D15:E15,"=X")*0.75</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="F16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="13">
         <f t="shared" ref="G16:G18" si="1">COUNTIF(D16:E16,"=X")*0.5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="25" t="s">
         <v>32</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1011,7 +1026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C18" s="7" t="s">
         <v>7</v>
       </c>
@@ -1029,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C19" s="7" t="s">
         <v>8</v>
       </c>
@@ -1047,7 +1062,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C20" s="22" t="s">
         <v>28</v>
       </c>
@@ -1058,10 +1073,10 @@
       </c>
       <c r="G20" s="12">
         <f>MIN(6,SUM(G15:G19))</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" ht="25.5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C21" s="1"/>
       <c r="D21" s="10" t="s">
         <v>16</v>
@@ -1076,7 +1091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C22" s="7" t="s">
         <v>10</v>
       </c>
@@ -1090,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C23" s="7" t="s">
         <v>12</v>
       </c>
@@ -1104,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C24" s="7" t="s">
         <v>14</v>
       </c>
@@ -1118,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C25" s="7" t="s">
         <v>15</v>
       </c>
@@ -1136,28 +1151,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
+      <c r="D26" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="31"/>
       <c r="F26" s="3">
         <v>0.5</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="3:7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="30"/>
+      <c r="D27" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="31"/>
       <c r="F27" s="3">
         <v>0.5</v>
       </c>
@@ -1166,12 +1183,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="3:7">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C28" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
       <c r="F28" s="3">
         <v>0.5</v>
       </c>
@@ -1180,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:7">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C29" s="22" t="s">
         <v>27</v>
       </c>
@@ -1191,19 +1208,19 @@
       </c>
       <c r="G29" s="12">
         <f>MIN(2,SUM(G23:G28))</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="30" spans="3:7">
-      <c r="C30" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C30" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30"/>
       <c r="G30" s="8">
         <f>MIN(10,SUM(G29,G20,G13))</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1219,7 +1236,7 @@
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.9055118110236221" right="0.9055118110236221" top="0.94488188976377963" bottom="0.94488188976377963" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>